<commit_message>
VehicleHandler #12 - Documentation - Update VehicleHandler TableStructure
</commit_message>
<xml_diff>
--- a/Documentation/VehicleHandlerTableStructure.xlsx
+++ b/Documentation/VehicleHandlerTableStructure.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="52">
   <si>
     <t>Vehicle</t>
   </si>
@@ -71,15 +71,6 @@
     <t>Blue</t>
   </si>
   <si>
-    <t>CustomVehicleColorsID1</t>
-  </si>
-  <si>
-    <t>ComponentColor1 Prio</t>
-  </si>
-  <si>
-    <t>ComponentColor2 Prio</t>
-  </si>
-  <si>
     <t>NumberplateValue</t>
   </si>
   <si>
@@ -98,9 +89,6 @@
     <t>Locked</t>
   </si>
   <si>
-    <t>FuelType</t>
-  </si>
-  <si>
     <t>EngineState</t>
   </si>
   <si>
@@ -128,20 +116,176 @@
     <t>TrunkDoorState</t>
   </si>
   <si>
-    <t>CustomVehicleColorsID2</t>
-  </si>
-  <si>
     <t>VehicleState</t>
   </si>
   <si>
     <t>Enum</t>
+  </si>
+  <si>
+    <t>Position</t>
+  </si>
+  <si>
+    <t>Rotation</t>
+  </si>
+  <si>
+    <t>Vector3</t>
+  </si>
+  <si>
+    <t>(unique)</t>
+  </si>
+  <si>
+    <t>PrimaryColorID</t>
+  </si>
+  <si>
+    <t>SecondaryColorID</t>
+  </si>
+  <si>
+    <t>{ComponentColor1 Prio}</t>
+  </si>
+  <si>
+    <t>{ComponentColor2 Prio}</t>
+  </si>
+  <si>
+    <t>VehicleProperties</t>
+  </si>
+  <si>
+    <r>
+      <t>Name</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FFD4D4D4"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>TankSize</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FFD4D4D4"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Consumption</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FFD4D4D4"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>TrunkSize</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FFD4D4D4"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>FuelType</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FFD4D4D4"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>DoorCount</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FFD4D4D4"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>TuningValue</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FFD4D4D4"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>BuildYear</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FFD4D4D4"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>MaxSpeed</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FFD4D4D4"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+  </si>
+  <si>
+    <t>Comment</t>
+  </si>
+  <si>
+    <t>VehicleClass</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -173,6 +317,12 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color rgb="FFD4D4D4"/>
+      <name val="Consolas"/>
+      <family val="3"/>
     </font>
     <font>
       <b/>
@@ -239,9 +389,9 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -522,120 +672,138 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:V31"/>
+  <dimension ref="A1:W33"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="D19" sqref="D19"/>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="F40" sqref="F40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="20.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="27.5703125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="14.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="4" width="30.7109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="18.140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="14.140625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="12.140625" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="10.5703125" customWidth="1"/>
-    <col min="15" max="15" width="17.140625" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="15.5703125" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="19.85546875" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="20" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="24.140625" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="15.140625" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="15.28515625" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="7.42578125" customWidth="1"/>
+    <col min="3" max="3" width="12" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="6" width="32.85546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="18.85546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="10" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="12" max="13" width="7.42578125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="10.5703125" customWidth="1"/>
+    <col min="16" max="16" width="17.140625" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="15.5703125" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="19.85546875" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="20" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="24.140625" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="15.140625" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="15.28515625" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="7.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:22" s="6" customFormat="1" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:23" s="6" customFormat="1" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
       <c r="C1" s="7" t="s">
-        <v>16</v>
+        <v>34</v>
       </c>
       <c r="D1" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="F1" s="6" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="2" spans="1:22" x14ac:dyDescent="0.25">
+        <v>34</v>
+      </c>
+      <c r="E1" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="F1" s="7" t="s">
+        <v>39</v>
+      </c>
+      <c r="G1" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="H1" s="7" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="2" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="B2" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="C2" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="G2" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="D2" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="E2" s="3" t="s">
+      <c r="H2" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="I2" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="J2" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="K2" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="F2" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="G2" s="3" t="s">
+      <c r="L2" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="H2" s="3" t="s">
+      <c r="M2" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="I2" s="3" t="s">
+      <c r="N2" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="J2" s="3" t="s">
+      <c r="O2" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="K2" s="3" t="s">
+      <c r="P2" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="L2" s="3" t="s">
+      <c r="Q2" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="M2" s="3" t="s">
+      <c r="R2" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="N2" s="3" t="s">
+      <c r="S2" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="O2" s="3" t="s">
+      <c r="T2" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="P2" s="3" t="s">
+      <c r="U2" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="Q2" s="3" t="s">
+      <c r="V2" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="R2" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="S2" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="T2" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="U2" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="V2" s="3"/>
-    </row>
-    <row r="3" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="W2" s="3"/>
+    </row>
+    <row r="3" spans="1:23" x14ac:dyDescent="0.25">
       <c r="B3" s="2"/>
     </row>
-    <row r="7" spans="1:22" s="6" customFormat="1" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="7" spans="1:23" s="6" customFormat="1" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A7" s="5" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
         <v>4</v>
       </c>
@@ -643,7 +811,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="9" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>1</v>
       </c>
@@ -651,7 +819,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="10" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>1</v>
       </c>
@@ -659,7 +827,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="11" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>2</v>
       </c>
@@ -667,7 +835,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="12" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>1</v>
       </c>
@@ -675,7 +843,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="13" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>6</v>
       </c>
@@ -683,12 +851,12 @@
         <v>3</v>
       </c>
     </row>
-    <row r="15" spans="1:22" s="6" customFormat="1" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="15" spans="1:23" s="6" customFormat="1" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A15" s="5" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="16" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
         <v>8</v>
       </c>
@@ -699,41 +867,69 @@
         <v>6</v>
       </c>
     </row>
-    <row r="22" spans="1:4" s="6" customFormat="1" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A22" s="5" t="s">
+    <row r="20" spans="1:4" s="6" customFormat="1" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A20" s="5" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A23" s="4" t="s">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A21" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="B23" s="4" t="s">
+      <c r="B21" s="4" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="27" spans="1:4" s="6" customFormat="1" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A27" s="5" t="s">
+    <row r="25" spans="1:4" s="6" customFormat="1" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A25" s="5" t="s">
         <v>10</v>
       </c>
     </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A26" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B26" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C26" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D26" s="2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A27">
+        <v>1</v>
+      </c>
+      <c r="B27">
+        <v>255</v>
+      </c>
+      <c r="C27">
+        <v>255</v>
+      </c>
+      <c r="D27">
+        <v>255</v>
+      </c>
+    </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A28" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="B28" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="C28" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="D28" s="2" t="s">
-        <v>14</v>
+      <c r="A28">
+        <v>2</v>
+      </c>
+      <c r="B28">
+        <v>1</v>
+      </c>
+      <c r="C28">
+        <v>1</v>
+      </c>
+      <c r="D28">
+        <v>1</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="B29">
         <v>255</v>
@@ -745,32 +941,50 @@
         <v>255</v>
       </c>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A30">
+    <row r="32" spans="1:4" s="6" customFormat="1" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A32" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="B32" s="7" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="33" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A33" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="B30">
-        <v>1</v>
-      </c>
-      <c r="C30">
-        <v>1</v>
-      </c>
-      <c r="D30">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A31">
-        <v>3</v>
-      </c>
-      <c r="B31">
-        <v>255</v>
-      </c>
-      <c r="C31">
-        <v>255</v>
-      </c>
-      <c r="D31">
-        <v>255</v>
+      <c r="B33" t="s">
+        <v>51</v>
+      </c>
+      <c r="C33" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="D33" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="E33" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="F33" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="G33" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="H33" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="I33" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="J33" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="K33" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="L33" s="3" t="s">
+        <v>50</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
VehicleHandler #12 -  Documentration - Permission VehicleUsers
</commit_message>
<xml_diff>
--- a/Documentation/VehicleHandlerTableStructure.xlsx
+++ b/Documentation/VehicleHandlerTableStructure.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="53">
   <si>
     <t>Vehicle</t>
   </si>
@@ -279,6 +279,9 @@
   </si>
   <si>
     <t>VehicleClass</t>
+  </si>
+  <si>
+    <t>Permission</t>
   </si>
 </sst>
 </file>
@@ -675,7 +678,7 @@
   <dimension ref="A1:W33"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="F12" sqref="F12"/>
+      <selection activeCell="O5" sqref="O5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -871,6 +874,9 @@
       <c r="A20" s="5" t="s">
         <v>9</v>
       </c>
+      <c r="C20" s="6" t="s">
+        <v>31</v>
+      </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" s="4" t="s">
@@ -878,6 +884,9 @@
       </c>
       <c r="B21" s="4" t="s">
         <v>3</v>
+      </c>
+      <c r="C21" t="s">
+        <v>52</v>
       </c>
     </row>
     <row r="25" spans="1:4" s="6" customFormat="1" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">

</xml_diff>

<commit_message>
VehicleHandler #12 - Zwischenstand VehicleHandler implementation
</commit_message>
<xml_diff>
--- a/Documentation/VehicleHandlerTableStructure.xlsx
+++ b/Documentation/VehicleHandlerTableStructure.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\#_Files\1_Programming\3_GitHub\EvoMpCore\Documentation\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\!_Files\1_Programming\3_GitHub\EvoMpCore\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="56">
   <si>
     <t>Vehicle</t>
   </si>
@@ -282,6 +282,15 @@
   </si>
   <si>
     <t>Permission</t>
+  </si>
+  <si>
+    <t>DoorStates</t>
+  </si>
+  <si>
+    <t>Door</t>
+  </si>
+  <si>
+    <t>State</t>
   </si>
 </sst>
 </file>
@@ -675,10 +684,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:W33"/>
+  <dimension ref="A1:W36"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="O5" sqref="O5"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -801,41 +810,45 @@
     <row r="3" spans="1:23" x14ac:dyDescent="0.25">
       <c r="B3" s="2"/>
     </row>
-    <row r="7" spans="1:23" s="6" customFormat="1" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A7" s="5" t="s">
+    <row r="5" spans="1:23" s="6" customFormat="1" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A5" s="5" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="6" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A6" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B6" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="C6" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="7" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A7" s="4"/>
+      <c r="B7" s="4"/>
+    </row>
+    <row r="8" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A8" s="4"/>
+      <c r="B8" s="4"/>
+    </row>
+    <row r="9" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A9" s="4"/>
+      <c r="B9" s="4"/>
+    </row>
+    <row r="10" spans="1:23" s="6" customFormat="1" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A10" s="5" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A8" s="4" t="s">
+    <row r="11" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A11" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="B8" s="4" t="s">
+      <c r="B11" s="4" t="s">
         <v>8</v>
-      </c>
-    </row>
-    <row r="9" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A9">
-        <v>1</v>
-      </c>
-      <c r="B9">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="10" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A10">
-        <v>1</v>
-      </c>
-      <c r="B10">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="11" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A11">
-        <v>2</v>
-      </c>
-      <c r="B11">
-        <v>3</v>
       </c>
     </row>
     <row r="12" spans="1:23" x14ac:dyDescent="0.25">
@@ -843,156 +856,180 @@
         <v>1</v>
       </c>
       <c r="B12">
-        <v>8</v>
+        <v>5</v>
       </c>
     </row>
     <row r="13" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A13">
+        <v>1</v>
+      </c>
+      <c r="B13">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="14" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>2</v>
+      </c>
+      <c r="B14">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="15" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>1</v>
+      </c>
+      <c r="B15">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="16" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A16">
         <v>6</v>
       </c>
-      <c r="B13">
+      <c r="B16">
         <v>3</v>
       </c>
     </row>
-    <row r="15" spans="1:23" s="6" customFormat="1" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A15" s="5" t="s">
+    <row r="18" spans="1:4" s="6" customFormat="1" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A18" s="5" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="16" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A16" s="2" t="s">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A19" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="B16" s="2" t="s">
+      <c r="B19" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C16" s="2" t="s">
+      <c r="C19" s="2" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="20" spans="1:4" s="6" customFormat="1" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A20" s="5" t="s">
+    <row r="23" spans="1:4" s="6" customFormat="1" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A23" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="C20" s="6" t="s">
+      <c r="C23" s="6" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A21" s="4" t="s">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A24" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="B21" s="4" t="s">
+      <c r="B24" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="C21" t="s">
+      <c r="C24" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="25" spans="1:4" s="6" customFormat="1" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A25" s="5" t="s">
+    <row r="28" spans="1:4" s="6" customFormat="1" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A28" s="5" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A26" s="2" t="s">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A29" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="B26" s="2" t="s">
+      <c r="B29" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="C26" s="2" t="s">
+      <c r="C29" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="D26" s="2" t="s">
+      <c r="D29" s="2" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A27">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A30">
         <v>1</v>
       </c>
-      <c r="B27">
+      <c r="B30">
         <v>255</v>
       </c>
-      <c r="C27">
+      <c r="C30">
         <v>255</v>
       </c>
-      <c r="D27">
+      <c r="D30">
         <v>255</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A28">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A31">
         <v>2</v>
       </c>
-      <c r="B28">
+      <c r="B31">
         <v>1</v>
       </c>
-      <c r="C28">
+      <c r="C31">
         <v>1</v>
       </c>
-      <c r="D28">
+      <c r="D31">
         <v>1</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A29">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A32">
         <v>3</v>
       </c>
-      <c r="B29">
+      <c r="B32">
         <v>255</v>
       </c>
-      <c r="C29">
+      <c r="C32">
         <v>255</v>
       </c>
-      <c r="D29">
+      <c r="D32">
         <v>255</v>
       </c>
     </row>
-    <row r="32" spans="1:4" s="6" customFormat="1" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A32" s="5" t="s">
+    <row r="35" spans="1:12" s="6" customFormat="1" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A35" s="5" t="s">
         <v>40</v>
       </c>
-      <c r="B32" s="7" t="s">
+      <c r="B35" s="7" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="33" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A33" s="4" t="s">
+    <row r="36" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A36" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="B33" t="s">
+      <c r="B36" t="s">
         <v>51</v>
       </c>
-      <c r="C33" s="3" t="s">
+      <c r="C36" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="D33" s="3" t="s">
+      <c r="D36" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="E33" s="3" t="s">
+      <c r="E36" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="F33" s="3" t="s">
+      <c r="F36" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="G33" s="3" t="s">
+      <c r="G36" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="H33" s="3" t="s">
+      <c r="H36" s="3" t="s">
         <v>46</v>
       </c>
-      <c r="I33" s="3" t="s">
+      <c r="I36" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="J33" s="3" t="s">
+      <c r="J36" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="K33" s="3" t="s">
+      <c r="K36" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="L33" s="3" t="s">
+      <c r="L36" s="3" t="s">
         <v>50</v>
       </c>
     </row>

</xml_diff>